<commit_message>
Updated for the script to add the JSON evidence data to the ComplianceFolder/ directory.
</commit_message>
<xml_diff>
--- a/NIST_to_SecOps.xlsx
+++ b/NIST_to_SecOps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://primusservices-my.sharepoint.com/personal/andrew_hamilton_cybriant_com/Documents/Programming/SecOps_Compliance_As_Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{4F0B36C5-4BD6-42BC-9416-8DCCBF291C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD2EAB26-686B-41A5-9790-B8E2C87CFA2C}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{4F0B36C5-4BD6-42BC-9416-8DCCBF291C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D5B7284-C7C9-4D7C-8F4F-D9F92B162120}"/>
   <bookViews>
-    <workbookView xWindow="-49125" yWindow="4035" windowWidth="45510" windowHeight="15120" xr2:uid="{B9B4F89A-A651-42E2-8F4E-447ADA8CBB1A}"/>
+    <workbookView xWindow="-42690" yWindow="885" windowWidth="35070" windowHeight="12015" xr2:uid="{B9B4F89A-A651-42E2-8F4E-447ADA8CBB1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -11807,20 +11807,20 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:R96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="L55" sqref="L55"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.140625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" customWidth="1"/>
     <col min="2" max="3" width="43.5703125" customWidth="1"/>
     <col min="4" max="5" width="31.85546875" customWidth="1"/>
     <col min="6" max="7" width="31" customWidth="1"/>
     <col min="8" max="8" width="25" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" style="10" customWidth="1"/>
+    <col min="9" max="9" width="26" style="10" customWidth="1"/>
     <col min="10" max="11" width="15.42578125" customWidth="1"/>
     <col min="12" max="12" width="37.7109375" style="14" customWidth="1"/>
     <col min="13" max="14" width="14.28515625" style="19" customWidth="1"/>

</xml_diff>